<commit_message>
feat: Add thermal data for 323,9х6,3 column in XLSX and JSON formats.
</commit_message>
<xml_diff>
--- a/thermal xlm/323,9х6,3.xlsx
+++ b/thermal xlm/323,9х6,3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\01_Postgraduate\Статьи\ВАК\ВАК Пожары и ЧС3 Сталебетон\Python program_V2\fire_column_app\thermal xlm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D841D253-8964-4D36-A86E-DE5C8A883C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB52615-FC54-4F5B-AAFF-1ECC5A622642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EEF9BC8-23BF-450E-9042-F798D29F0F82}"/>
   </bookViews>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EB8B82-DEFF-4CFC-9AAE-C98B3F9C19FD}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:J242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,6 +3368,4806 @@
         <v>130.75</v>
       </c>
     </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>5460</v>
+      </c>
+      <c r="B93">
+        <v>941.41</v>
+      </c>
+      <c r="C93">
+        <v>858.92</v>
+      </c>
+      <c r="D93">
+        <v>653.33000000000004</v>
+      </c>
+      <c r="E93">
+        <v>475.17</v>
+      </c>
+      <c r="F93">
+        <v>475.17</v>
+      </c>
+      <c r="G93">
+        <v>355.51</v>
+      </c>
+      <c r="H93">
+        <v>261.5</v>
+      </c>
+      <c r="I93">
+        <v>194.89</v>
+      </c>
+      <c r="J93">
+        <v>132.93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>5520</v>
+      </c>
+      <c r="B94">
+        <v>943.62</v>
+      </c>
+      <c r="C94">
+        <v>861.59</v>
+      </c>
+      <c r="D94">
+        <v>656.72</v>
+      </c>
+      <c r="E94">
+        <v>478.78</v>
+      </c>
+      <c r="F94">
+        <v>478.78</v>
+      </c>
+      <c r="G94">
+        <v>359.06</v>
+      </c>
+      <c r="H94">
+        <v>264.94</v>
+      </c>
+      <c r="I94">
+        <v>198.24</v>
+      </c>
+      <c r="J94">
+        <v>135.19999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>5580</v>
+      </c>
+      <c r="B95">
+        <v>945.79</v>
+      </c>
+      <c r="C95">
+        <v>864.22</v>
+      </c>
+      <c r="D95">
+        <v>660.08</v>
+      </c>
+      <c r="E95">
+        <v>482.35</v>
+      </c>
+      <c r="F95">
+        <v>482.35</v>
+      </c>
+      <c r="G95">
+        <v>362.59</v>
+      </c>
+      <c r="H95">
+        <v>268.37</v>
+      </c>
+      <c r="I95">
+        <v>201.59</v>
+      </c>
+      <c r="J95">
+        <v>137.55000000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>5640</v>
+      </c>
+      <c r="B96">
+        <v>947.93</v>
+      </c>
+      <c r="C96">
+        <v>866.82</v>
+      </c>
+      <c r="D96">
+        <v>663.4</v>
+      </c>
+      <c r="E96">
+        <v>485.9</v>
+      </c>
+      <c r="F96">
+        <v>485.9</v>
+      </c>
+      <c r="G96">
+        <v>366.1</v>
+      </c>
+      <c r="H96">
+        <v>271.79000000000002</v>
+      </c>
+      <c r="I96">
+        <v>204.94</v>
+      </c>
+      <c r="J96">
+        <v>139.99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>5700</v>
+      </c>
+      <c r="B97">
+        <v>950.05</v>
+      </c>
+      <c r="C97">
+        <v>869.39</v>
+      </c>
+      <c r="D97">
+        <v>666.68</v>
+      </c>
+      <c r="E97">
+        <v>489.41</v>
+      </c>
+      <c r="F97">
+        <v>489.41</v>
+      </c>
+      <c r="G97">
+        <v>369.58</v>
+      </c>
+      <c r="H97">
+        <v>275.18</v>
+      </c>
+      <c r="I97">
+        <v>208.29</v>
+      </c>
+      <c r="J97">
+        <v>142.52000000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>5760</v>
+      </c>
+      <c r="B98">
+        <v>952.13</v>
+      </c>
+      <c r="C98">
+        <v>871.92</v>
+      </c>
+      <c r="D98">
+        <v>669.93</v>
+      </c>
+      <c r="E98">
+        <v>492.9</v>
+      </c>
+      <c r="F98">
+        <v>492.9</v>
+      </c>
+      <c r="G98">
+        <v>373.04</v>
+      </c>
+      <c r="H98">
+        <v>278.57</v>
+      </c>
+      <c r="I98">
+        <v>211.64</v>
+      </c>
+      <c r="J98">
+        <v>145.13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>5820</v>
+      </c>
+      <c r="B99">
+        <v>954.19</v>
+      </c>
+      <c r="C99">
+        <v>874.42</v>
+      </c>
+      <c r="D99">
+        <v>673.15</v>
+      </c>
+      <c r="E99">
+        <v>496.36</v>
+      </c>
+      <c r="F99">
+        <v>496.36</v>
+      </c>
+      <c r="G99">
+        <v>376.48</v>
+      </c>
+      <c r="H99">
+        <v>281.93</v>
+      </c>
+      <c r="I99">
+        <v>214.99</v>
+      </c>
+      <c r="J99">
+        <v>147.83000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>5880</v>
+      </c>
+      <c r="B100">
+        <v>956.22</v>
+      </c>
+      <c r="C100">
+        <v>876.89</v>
+      </c>
+      <c r="D100">
+        <v>676.34</v>
+      </c>
+      <c r="E100">
+        <v>499.8</v>
+      </c>
+      <c r="F100">
+        <v>499.8</v>
+      </c>
+      <c r="G100">
+        <v>379.9</v>
+      </c>
+      <c r="H100">
+        <v>285.29000000000002</v>
+      </c>
+      <c r="I100">
+        <v>218.33</v>
+      </c>
+      <c r="J100">
+        <v>150.62</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>5940</v>
+      </c>
+      <c r="B101">
+        <v>958.22</v>
+      </c>
+      <c r="C101">
+        <v>879.33</v>
+      </c>
+      <c r="D101">
+        <v>679.5</v>
+      </c>
+      <c r="E101">
+        <v>503.2</v>
+      </c>
+      <c r="F101">
+        <v>503.2</v>
+      </c>
+      <c r="G101">
+        <v>383.3</v>
+      </c>
+      <c r="H101">
+        <v>288.63</v>
+      </c>
+      <c r="I101">
+        <v>221.66</v>
+      </c>
+      <c r="J101">
+        <v>153.5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>6000</v>
+      </c>
+      <c r="B102">
+        <v>960.2</v>
+      </c>
+      <c r="C102">
+        <v>881.74</v>
+      </c>
+      <c r="D102">
+        <v>682.62</v>
+      </c>
+      <c r="E102">
+        <v>506.58</v>
+      </c>
+      <c r="F102">
+        <v>506.58</v>
+      </c>
+      <c r="G102">
+        <v>386.67</v>
+      </c>
+      <c r="H102">
+        <v>291.95</v>
+      </c>
+      <c r="I102">
+        <v>224.99</v>
+      </c>
+      <c r="J102">
+        <v>156.47</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>6060</v>
+      </c>
+      <c r="B103">
+        <v>962.15</v>
+      </c>
+      <c r="C103">
+        <v>884.12</v>
+      </c>
+      <c r="D103">
+        <v>685.72</v>
+      </c>
+      <c r="E103">
+        <v>509.93</v>
+      </c>
+      <c r="F103">
+        <v>509.93</v>
+      </c>
+      <c r="G103">
+        <v>390.03</v>
+      </c>
+      <c r="H103">
+        <v>295.27</v>
+      </c>
+      <c r="I103">
+        <v>228.32</v>
+      </c>
+      <c r="J103">
+        <v>159.53</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>6120</v>
+      </c>
+      <c r="B104">
+        <v>964.08</v>
+      </c>
+      <c r="C104">
+        <v>886.48</v>
+      </c>
+      <c r="D104">
+        <v>688.78</v>
+      </c>
+      <c r="E104">
+        <v>513.26</v>
+      </c>
+      <c r="F104">
+        <v>513.26</v>
+      </c>
+      <c r="G104">
+        <v>393.37</v>
+      </c>
+      <c r="H104">
+        <v>298.57</v>
+      </c>
+      <c r="I104">
+        <v>231.65</v>
+      </c>
+      <c r="J104">
+        <v>162.66999999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>6180</v>
+      </c>
+      <c r="B105">
+        <v>965.99</v>
+      </c>
+      <c r="C105">
+        <v>888.8</v>
+      </c>
+      <c r="D105">
+        <v>691.82</v>
+      </c>
+      <c r="E105">
+        <v>516.55999999999995</v>
+      </c>
+      <c r="F105">
+        <v>516.55999999999995</v>
+      </c>
+      <c r="G105">
+        <v>396.69</v>
+      </c>
+      <c r="H105">
+        <v>301.86</v>
+      </c>
+      <c r="I105">
+        <v>234.96</v>
+      </c>
+      <c r="J105">
+        <v>165.91</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>6240</v>
+      </c>
+      <c r="B106">
+        <v>967.87</v>
+      </c>
+      <c r="C106">
+        <v>891.1</v>
+      </c>
+      <c r="D106">
+        <v>694.83</v>
+      </c>
+      <c r="E106">
+        <v>519.84</v>
+      </c>
+      <c r="F106">
+        <v>519.84</v>
+      </c>
+      <c r="G106">
+        <v>399.99</v>
+      </c>
+      <c r="H106">
+        <v>305.13</v>
+      </c>
+      <c r="I106">
+        <v>238.28</v>
+      </c>
+      <c r="J106">
+        <v>169.23</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>6300</v>
+      </c>
+      <c r="B107">
+        <v>969.73</v>
+      </c>
+      <c r="C107">
+        <v>893.38</v>
+      </c>
+      <c r="D107">
+        <v>697.81</v>
+      </c>
+      <c r="E107">
+        <v>523.09</v>
+      </c>
+      <c r="F107">
+        <v>523.09</v>
+      </c>
+      <c r="G107">
+        <v>403.27</v>
+      </c>
+      <c r="H107">
+        <v>308.39999999999998</v>
+      </c>
+      <c r="I107">
+        <v>241.59</v>
+      </c>
+      <c r="J107">
+        <v>172.65</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>6360</v>
+      </c>
+      <c r="B108">
+        <v>971.56</v>
+      </c>
+      <c r="C108">
+        <v>895.63</v>
+      </c>
+      <c r="D108">
+        <v>700.76</v>
+      </c>
+      <c r="E108">
+        <v>526.30999999999995</v>
+      </c>
+      <c r="F108">
+        <v>526.30999999999995</v>
+      </c>
+      <c r="G108">
+        <v>406.54</v>
+      </c>
+      <c r="H108">
+        <v>311.64999999999998</v>
+      </c>
+      <c r="I108">
+        <v>244.9</v>
+      </c>
+      <c r="J108">
+        <v>176.14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>6420</v>
+      </c>
+      <c r="B109">
+        <v>973.38</v>
+      </c>
+      <c r="C109">
+        <v>897.85</v>
+      </c>
+      <c r="D109">
+        <v>703.69</v>
+      </c>
+      <c r="E109">
+        <v>529.52</v>
+      </c>
+      <c r="F109">
+        <v>529.52</v>
+      </c>
+      <c r="G109">
+        <v>409.79</v>
+      </c>
+      <c r="H109">
+        <v>314.89</v>
+      </c>
+      <c r="I109">
+        <v>248.21</v>
+      </c>
+      <c r="J109">
+        <v>179.72</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>6480</v>
+      </c>
+      <c r="B110">
+        <v>975.17</v>
+      </c>
+      <c r="C110">
+        <v>900.06</v>
+      </c>
+      <c r="D110">
+        <v>706.59</v>
+      </c>
+      <c r="E110">
+        <v>532.69000000000005</v>
+      </c>
+      <c r="F110">
+        <v>532.69000000000005</v>
+      </c>
+      <c r="G110">
+        <v>413.02</v>
+      </c>
+      <c r="H110">
+        <v>318.12</v>
+      </c>
+      <c r="I110">
+        <v>251.51</v>
+      </c>
+      <c r="J110">
+        <v>183.38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>6540</v>
+      </c>
+      <c r="B111">
+        <v>976.94</v>
+      </c>
+      <c r="C111">
+        <v>902.23</v>
+      </c>
+      <c r="D111">
+        <v>709.47</v>
+      </c>
+      <c r="E111">
+        <v>535.85</v>
+      </c>
+      <c r="F111">
+        <v>535.85</v>
+      </c>
+      <c r="G111">
+        <v>416.23</v>
+      </c>
+      <c r="H111">
+        <v>321.33999999999997</v>
+      </c>
+      <c r="I111">
+        <v>254.8</v>
+      </c>
+      <c r="J111">
+        <v>187.1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>6600</v>
+      </c>
+      <c r="B112">
+        <v>978.7</v>
+      </c>
+      <c r="C112">
+        <v>904.39</v>
+      </c>
+      <c r="D112">
+        <v>712.32</v>
+      </c>
+      <c r="E112">
+        <v>538.98</v>
+      </c>
+      <c r="F112">
+        <v>538.98</v>
+      </c>
+      <c r="G112">
+        <v>419.42</v>
+      </c>
+      <c r="H112">
+        <v>324.54000000000002</v>
+      </c>
+      <c r="I112">
+        <v>258.10000000000002</v>
+      </c>
+      <c r="J112">
+        <v>190.89</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>6660</v>
+      </c>
+      <c r="B113">
+        <v>980.43</v>
+      </c>
+      <c r="C113">
+        <v>906.51</v>
+      </c>
+      <c r="D113">
+        <v>715.14</v>
+      </c>
+      <c r="E113">
+        <v>542.1</v>
+      </c>
+      <c r="F113">
+        <v>542.1</v>
+      </c>
+      <c r="G113">
+        <v>422.6</v>
+      </c>
+      <c r="H113">
+        <v>327.74</v>
+      </c>
+      <c r="I113">
+        <v>261.39</v>
+      </c>
+      <c r="J113">
+        <v>194.72</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>6720</v>
+      </c>
+      <c r="B114">
+        <v>982.15</v>
+      </c>
+      <c r="C114">
+        <v>908.61</v>
+      </c>
+      <c r="D114">
+        <v>717.94</v>
+      </c>
+      <c r="E114">
+        <v>545.17999999999995</v>
+      </c>
+      <c r="F114">
+        <v>545.17999999999995</v>
+      </c>
+      <c r="G114">
+        <v>425.76</v>
+      </c>
+      <c r="H114">
+        <v>330.92</v>
+      </c>
+      <c r="I114">
+        <v>264.67</v>
+      </c>
+      <c r="J114">
+        <v>198.58</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>6780</v>
+      </c>
+      <c r="B115">
+        <v>983.84</v>
+      </c>
+      <c r="C115">
+        <v>910.7</v>
+      </c>
+      <c r="D115">
+        <v>720.72</v>
+      </c>
+      <c r="E115">
+        <v>548.25</v>
+      </c>
+      <c r="F115">
+        <v>548.25</v>
+      </c>
+      <c r="G115">
+        <v>428.91</v>
+      </c>
+      <c r="H115">
+        <v>334.09</v>
+      </c>
+      <c r="I115">
+        <v>267.95</v>
+      </c>
+      <c r="J115">
+        <v>202.46</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>6840</v>
+      </c>
+      <c r="B116">
+        <v>985.52</v>
+      </c>
+      <c r="C116">
+        <v>912.76</v>
+      </c>
+      <c r="D116">
+        <v>723.47</v>
+      </c>
+      <c r="E116">
+        <v>551.29999999999995</v>
+      </c>
+      <c r="F116">
+        <v>551.29999999999995</v>
+      </c>
+      <c r="G116">
+        <v>432.03</v>
+      </c>
+      <c r="H116">
+        <v>337.25</v>
+      </c>
+      <c r="I116">
+        <v>271.23</v>
+      </c>
+      <c r="J116">
+        <v>206.35</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>6900</v>
+      </c>
+      <c r="B117">
+        <v>987.18</v>
+      </c>
+      <c r="C117">
+        <v>914.8</v>
+      </c>
+      <c r="D117">
+        <v>726.19</v>
+      </c>
+      <c r="E117">
+        <v>554.33000000000004</v>
+      </c>
+      <c r="F117">
+        <v>554.33000000000004</v>
+      </c>
+      <c r="G117">
+        <v>435.15</v>
+      </c>
+      <c r="H117">
+        <v>340.4</v>
+      </c>
+      <c r="I117">
+        <v>274.5</v>
+      </c>
+      <c r="J117">
+        <v>210.23</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>6960</v>
+      </c>
+      <c r="B118">
+        <v>988.82</v>
+      </c>
+      <c r="C118">
+        <v>916.82</v>
+      </c>
+      <c r="D118">
+        <v>728.89</v>
+      </c>
+      <c r="E118">
+        <v>557.34</v>
+      </c>
+      <c r="F118">
+        <v>557.34</v>
+      </c>
+      <c r="G118">
+        <v>438.24</v>
+      </c>
+      <c r="H118">
+        <v>343.55</v>
+      </c>
+      <c r="I118">
+        <v>277.76</v>
+      </c>
+      <c r="J118">
+        <v>214.08</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>7020</v>
+      </c>
+      <c r="B119">
+        <v>990.44</v>
+      </c>
+      <c r="C119">
+        <v>918.81</v>
+      </c>
+      <c r="D119">
+        <v>731.57</v>
+      </c>
+      <c r="E119">
+        <v>560.33000000000004</v>
+      </c>
+      <c r="F119">
+        <v>560.33000000000004</v>
+      </c>
+      <c r="G119">
+        <v>441.33</v>
+      </c>
+      <c r="H119">
+        <v>346.68</v>
+      </c>
+      <c r="I119">
+        <v>281.01</v>
+      </c>
+      <c r="J119">
+        <v>217.89</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>7080</v>
+      </c>
+      <c r="B120">
+        <v>992.05</v>
+      </c>
+      <c r="C120">
+        <v>920.79</v>
+      </c>
+      <c r="D120">
+        <v>734.23</v>
+      </c>
+      <c r="E120">
+        <v>563.29</v>
+      </c>
+      <c r="F120">
+        <v>563.29</v>
+      </c>
+      <c r="G120">
+        <v>444.39</v>
+      </c>
+      <c r="H120">
+        <v>349.79</v>
+      </c>
+      <c r="I120">
+        <v>284.26</v>
+      </c>
+      <c r="J120">
+        <v>221.66</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>7140</v>
+      </c>
+      <c r="B121">
+        <v>993.64</v>
+      </c>
+      <c r="C121">
+        <v>922.74</v>
+      </c>
+      <c r="D121">
+        <v>736.87</v>
+      </c>
+      <c r="E121">
+        <v>566.24</v>
+      </c>
+      <c r="F121">
+        <v>566.24</v>
+      </c>
+      <c r="G121">
+        <v>447.45</v>
+      </c>
+      <c r="H121">
+        <v>352.9</v>
+      </c>
+      <c r="I121">
+        <v>287.49</v>
+      </c>
+      <c r="J121">
+        <v>225.37</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>7200</v>
+      </c>
+      <c r="B122">
+        <v>995.22</v>
+      </c>
+      <c r="C122">
+        <v>924.68</v>
+      </c>
+      <c r="D122">
+        <v>739.48</v>
+      </c>
+      <c r="E122">
+        <v>569.17999999999995</v>
+      </c>
+      <c r="F122">
+        <v>569.17999999999995</v>
+      </c>
+      <c r="G122">
+        <v>450.49</v>
+      </c>
+      <c r="H122">
+        <v>356</v>
+      </c>
+      <c r="I122">
+        <v>290.72000000000003</v>
+      </c>
+      <c r="J122">
+        <v>229.04</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>7260</v>
+      </c>
+      <c r="B123">
+        <v>996.77</v>
+      </c>
+      <c r="C123">
+        <v>926.59</v>
+      </c>
+      <c r="D123">
+        <v>742.07</v>
+      </c>
+      <c r="E123">
+        <v>572.09</v>
+      </c>
+      <c r="F123">
+        <v>572.09</v>
+      </c>
+      <c r="G123">
+        <v>453.51</v>
+      </c>
+      <c r="H123">
+        <v>359.09</v>
+      </c>
+      <c r="I123">
+        <v>293.94</v>
+      </c>
+      <c r="J123">
+        <v>232.66</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>7320</v>
+      </c>
+      <c r="B124">
+        <v>998.32</v>
+      </c>
+      <c r="C124">
+        <v>928.49</v>
+      </c>
+      <c r="D124">
+        <v>744.65</v>
+      </c>
+      <c r="E124">
+        <v>574.99</v>
+      </c>
+      <c r="F124">
+        <v>574.99</v>
+      </c>
+      <c r="G124">
+        <v>456.52</v>
+      </c>
+      <c r="H124">
+        <v>362.17</v>
+      </c>
+      <c r="I124">
+        <v>297.14</v>
+      </c>
+      <c r="J124">
+        <v>236.23</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>7380</v>
+      </c>
+      <c r="B125">
+        <v>999.84</v>
+      </c>
+      <c r="C125">
+        <v>930.37</v>
+      </c>
+      <c r="D125">
+        <v>747.2</v>
+      </c>
+      <c r="E125">
+        <v>577.87</v>
+      </c>
+      <c r="F125">
+        <v>577.87</v>
+      </c>
+      <c r="G125">
+        <v>459.52</v>
+      </c>
+      <c r="H125">
+        <v>365.24</v>
+      </c>
+      <c r="I125">
+        <v>300.33</v>
+      </c>
+      <c r="J125">
+        <v>239.75</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>7440</v>
+      </c>
+      <c r="B126">
+        <v>1001.4</v>
+      </c>
+      <c r="C126">
+        <v>932.23</v>
+      </c>
+      <c r="D126">
+        <v>749.73</v>
+      </c>
+      <c r="E126">
+        <v>580.73</v>
+      </c>
+      <c r="F126">
+        <v>580.73</v>
+      </c>
+      <c r="G126">
+        <v>462.5</v>
+      </c>
+      <c r="H126">
+        <v>368.29</v>
+      </c>
+      <c r="I126">
+        <v>303.51</v>
+      </c>
+      <c r="J126">
+        <v>243.24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>7500</v>
+      </c>
+      <c r="B127">
+        <v>1002.9</v>
+      </c>
+      <c r="C127">
+        <v>934.08</v>
+      </c>
+      <c r="D127">
+        <v>752.24</v>
+      </c>
+      <c r="E127">
+        <v>583.58000000000004</v>
+      </c>
+      <c r="F127">
+        <v>583.58000000000004</v>
+      </c>
+      <c r="G127">
+        <v>465.47</v>
+      </c>
+      <c r="H127">
+        <v>371.34</v>
+      </c>
+      <c r="I127">
+        <v>306.67</v>
+      </c>
+      <c r="J127">
+        <v>246.68</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>7560</v>
+      </c>
+      <c r="B128">
+        <v>1004.3</v>
+      </c>
+      <c r="C128">
+        <v>935.9</v>
+      </c>
+      <c r="D128">
+        <v>754.74</v>
+      </c>
+      <c r="E128">
+        <v>586.41</v>
+      </c>
+      <c r="F128">
+        <v>586.41</v>
+      </c>
+      <c r="G128">
+        <v>468.43</v>
+      </c>
+      <c r="H128">
+        <v>374.37</v>
+      </c>
+      <c r="I128">
+        <v>309.82</v>
+      </c>
+      <c r="J128">
+        <v>250.08</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>7620</v>
+      </c>
+      <c r="B129">
+        <v>1005.8</v>
+      </c>
+      <c r="C129">
+        <v>937.71</v>
+      </c>
+      <c r="D129">
+        <v>757.21</v>
+      </c>
+      <c r="E129">
+        <v>589.22</v>
+      </c>
+      <c r="F129">
+        <v>589.22</v>
+      </c>
+      <c r="G129">
+        <v>471.38</v>
+      </c>
+      <c r="H129">
+        <v>377.39</v>
+      </c>
+      <c r="I129">
+        <v>312.95999999999998</v>
+      </c>
+      <c r="J129">
+        <v>253.45</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>7680</v>
+      </c>
+      <c r="B130">
+        <v>1007.3</v>
+      </c>
+      <c r="C130">
+        <v>939.5</v>
+      </c>
+      <c r="D130">
+        <v>759.67</v>
+      </c>
+      <c r="E130">
+        <v>592.02</v>
+      </c>
+      <c r="F130">
+        <v>592.02</v>
+      </c>
+      <c r="G130">
+        <v>474.31</v>
+      </c>
+      <c r="H130">
+        <v>380.4</v>
+      </c>
+      <c r="I130">
+        <v>316.07</v>
+      </c>
+      <c r="J130">
+        <v>256.79000000000002</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>7740</v>
+      </c>
+      <c r="B131">
+        <v>1008.7</v>
+      </c>
+      <c r="C131">
+        <v>941.28</v>
+      </c>
+      <c r="D131">
+        <v>762.11</v>
+      </c>
+      <c r="E131">
+        <v>594.79999999999995</v>
+      </c>
+      <c r="F131">
+        <v>594.79999999999995</v>
+      </c>
+      <c r="G131">
+        <v>477.23</v>
+      </c>
+      <c r="H131">
+        <v>383.4</v>
+      </c>
+      <c r="I131">
+        <v>319.18</v>
+      </c>
+      <c r="J131">
+        <v>260.08999999999997</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>7800</v>
+      </c>
+      <c r="B132">
+        <v>1010.1</v>
+      </c>
+      <c r="C132">
+        <v>943.04</v>
+      </c>
+      <c r="D132">
+        <v>764.53</v>
+      </c>
+      <c r="E132">
+        <v>597.57000000000005</v>
+      </c>
+      <c r="F132">
+        <v>597.57000000000005</v>
+      </c>
+      <c r="G132">
+        <v>480.13</v>
+      </c>
+      <c r="H132">
+        <v>386.39</v>
+      </c>
+      <c r="I132">
+        <v>322.26</v>
+      </c>
+      <c r="J132">
+        <v>263.36</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>7860</v>
+      </c>
+      <c r="B133">
+        <v>1011.5</v>
+      </c>
+      <c r="C133">
+        <v>944.79</v>
+      </c>
+      <c r="D133">
+        <v>766.93</v>
+      </c>
+      <c r="E133">
+        <v>600.32000000000005</v>
+      </c>
+      <c r="F133">
+        <v>600.32000000000005</v>
+      </c>
+      <c r="G133">
+        <v>483.02</v>
+      </c>
+      <c r="H133">
+        <v>389.37</v>
+      </c>
+      <c r="I133">
+        <v>325.33</v>
+      </c>
+      <c r="J133">
+        <v>266.61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>7920</v>
+      </c>
+      <c r="B134">
+        <v>1012.9</v>
+      </c>
+      <c r="C134">
+        <v>946.52</v>
+      </c>
+      <c r="D134">
+        <v>769.32</v>
+      </c>
+      <c r="E134">
+        <v>603.05999999999995</v>
+      </c>
+      <c r="F134">
+        <v>603.05999999999995</v>
+      </c>
+      <c r="G134">
+        <v>485.9</v>
+      </c>
+      <c r="H134">
+        <v>392.33</v>
+      </c>
+      <c r="I134">
+        <v>328.38</v>
+      </c>
+      <c r="J134">
+        <v>269.82</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>7980</v>
+      </c>
+      <c r="B135">
+        <v>1014.3</v>
+      </c>
+      <c r="C135">
+        <v>948.23</v>
+      </c>
+      <c r="D135">
+        <v>771.69</v>
+      </c>
+      <c r="E135">
+        <v>605.78</v>
+      </c>
+      <c r="F135">
+        <v>605.78</v>
+      </c>
+      <c r="G135">
+        <v>488.77</v>
+      </c>
+      <c r="H135">
+        <v>395.28</v>
+      </c>
+      <c r="I135">
+        <v>331.42</v>
+      </c>
+      <c r="J135">
+        <v>273.01</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>8040</v>
+      </c>
+      <c r="B136">
+        <v>1015.7</v>
+      </c>
+      <c r="C136">
+        <v>949.93</v>
+      </c>
+      <c r="D136">
+        <v>774.04</v>
+      </c>
+      <c r="E136">
+        <v>608.49</v>
+      </c>
+      <c r="F136">
+        <v>608.49</v>
+      </c>
+      <c r="G136">
+        <v>491.63</v>
+      </c>
+      <c r="H136">
+        <v>398.23</v>
+      </c>
+      <c r="I136">
+        <v>334.44</v>
+      </c>
+      <c r="J136">
+        <v>276.18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>8100</v>
+      </c>
+      <c r="B137">
+        <v>1017.1</v>
+      </c>
+      <c r="C137">
+        <v>951.62</v>
+      </c>
+      <c r="D137">
+        <v>776.38</v>
+      </c>
+      <c r="E137">
+        <v>611.17999999999995</v>
+      </c>
+      <c r="F137">
+        <v>611.17999999999995</v>
+      </c>
+      <c r="G137">
+        <v>494.47</v>
+      </c>
+      <c r="H137">
+        <v>401.16</v>
+      </c>
+      <c r="I137">
+        <v>337.44</v>
+      </c>
+      <c r="J137">
+        <v>279.31</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>8160</v>
+      </c>
+      <c r="B138">
+        <v>1018.4</v>
+      </c>
+      <c r="C138">
+        <v>953.29</v>
+      </c>
+      <c r="D138">
+        <v>778.7</v>
+      </c>
+      <c r="E138">
+        <v>613.85</v>
+      </c>
+      <c r="F138">
+        <v>613.85</v>
+      </c>
+      <c r="G138">
+        <v>497.3</v>
+      </c>
+      <c r="H138">
+        <v>404.07</v>
+      </c>
+      <c r="I138">
+        <v>340.43</v>
+      </c>
+      <c r="J138">
+        <v>282.43</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>8220</v>
+      </c>
+      <c r="B139">
+        <v>1019.8</v>
+      </c>
+      <c r="C139">
+        <v>954.95</v>
+      </c>
+      <c r="D139">
+        <v>781.01</v>
+      </c>
+      <c r="E139">
+        <v>616.52</v>
+      </c>
+      <c r="F139">
+        <v>616.52</v>
+      </c>
+      <c r="G139">
+        <v>500.12</v>
+      </c>
+      <c r="H139">
+        <v>406.98</v>
+      </c>
+      <c r="I139">
+        <v>343.41</v>
+      </c>
+      <c r="J139">
+        <v>285.52</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>8280</v>
+      </c>
+      <c r="B140">
+        <v>1021.1</v>
+      </c>
+      <c r="C140">
+        <v>956.59</v>
+      </c>
+      <c r="D140">
+        <v>783.3</v>
+      </c>
+      <c r="E140">
+        <v>619.16</v>
+      </c>
+      <c r="F140">
+        <v>619.16</v>
+      </c>
+      <c r="G140">
+        <v>502.93</v>
+      </c>
+      <c r="H140">
+        <v>409.87</v>
+      </c>
+      <c r="I140">
+        <v>346.36</v>
+      </c>
+      <c r="J140">
+        <v>288.58999999999997</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>8340</v>
+      </c>
+      <c r="B141">
+        <v>1022.4</v>
+      </c>
+      <c r="C141">
+        <v>958.22</v>
+      </c>
+      <c r="D141">
+        <v>785.58</v>
+      </c>
+      <c r="E141">
+        <v>621.79999999999995</v>
+      </c>
+      <c r="F141">
+        <v>621.79999999999995</v>
+      </c>
+      <c r="G141">
+        <v>505.72</v>
+      </c>
+      <c r="H141">
+        <v>412.75</v>
+      </c>
+      <c r="I141">
+        <v>349.3</v>
+      </c>
+      <c r="J141">
+        <v>291.64</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>8400</v>
+      </c>
+      <c r="B142">
+        <v>1023.7</v>
+      </c>
+      <c r="C142">
+        <v>959.84</v>
+      </c>
+      <c r="D142">
+        <v>787.84</v>
+      </c>
+      <c r="E142">
+        <v>624.41999999999996</v>
+      </c>
+      <c r="F142">
+        <v>624.41999999999996</v>
+      </c>
+      <c r="G142">
+        <v>508.5</v>
+      </c>
+      <c r="H142">
+        <v>415.62</v>
+      </c>
+      <c r="I142">
+        <v>352.23</v>
+      </c>
+      <c r="J142">
+        <v>294.66000000000003</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>8460</v>
+      </c>
+      <c r="B143">
+        <v>1025</v>
+      </c>
+      <c r="C143">
+        <v>961.45</v>
+      </c>
+      <c r="D143">
+        <v>790.09</v>
+      </c>
+      <c r="E143">
+        <v>627.02</v>
+      </c>
+      <c r="F143">
+        <v>627.02</v>
+      </c>
+      <c r="G143">
+        <v>511.26</v>
+      </c>
+      <c r="H143">
+        <v>418.47</v>
+      </c>
+      <c r="I143">
+        <v>355.14</v>
+      </c>
+      <c r="J143">
+        <v>297.67</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>8520</v>
+      </c>
+      <c r="B144">
+        <v>1026.3</v>
+      </c>
+      <c r="C144">
+        <v>963.04</v>
+      </c>
+      <c r="D144">
+        <v>792.32</v>
+      </c>
+      <c r="E144">
+        <v>629.61</v>
+      </c>
+      <c r="F144">
+        <v>629.61</v>
+      </c>
+      <c r="G144">
+        <v>514.02</v>
+      </c>
+      <c r="H144">
+        <v>421.32</v>
+      </c>
+      <c r="I144">
+        <v>358.04</v>
+      </c>
+      <c r="J144">
+        <v>300.66000000000003</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>8580</v>
+      </c>
+      <c r="B145">
+        <v>1027.5999999999999</v>
+      </c>
+      <c r="C145">
+        <v>964.62</v>
+      </c>
+      <c r="D145">
+        <v>794.54</v>
+      </c>
+      <c r="E145">
+        <v>632.17999999999995</v>
+      </c>
+      <c r="F145">
+        <v>632.17999999999995</v>
+      </c>
+      <c r="G145">
+        <v>516.76</v>
+      </c>
+      <c r="H145">
+        <v>424.14</v>
+      </c>
+      <c r="I145">
+        <v>360.92</v>
+      </c>
+      <c r="J145">
+        <v>303.62</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>8640</v>
+      </c>
+      <c r="B146">
+        <v>1028.9000000000001</v>
+      </c>
+      <c r="C146">
+        <v>966.19</v>
+      </c>
+      <c r="D146">
+        <v>796.74</v>
+      </c>
+      <c r="E146">
+        <v>634.75</v>
+      </c>
+      <c r="F146">
+        <v>634.75</v>
+      </c>
+      <c r="G146">
+        <v>519.49</v>
+      </c>
+      <c r="H146">
+        <v>426.96</v>
+      </c>
+      <c r="I146">
+        <v>363.79</v>
+      </c>
+      <c r="J146">
+        <v>306.57</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>8700</v>
+      </c>
+      <c r="B147">
+        <v>1030.0999999999999</v>
+      </c>
+      <c r="C147">
+        <v>967.74</v>
+      </c>
+      <c r="D147">
+        <v>798.93</v>
+      </c>
+      <c r="E147">
+        <v>637.29</v>
+      </c>
+      <c r="F147">
+        <v>637.29</v>
+      </c>
+      <c r="G147">
+        <v>522.20000000000005</v>
+      </c>
+      <c r="H147">
+        <v>429.76</v>
+      </c>
+      <c r="I147">
+        <v>366.64</v>
+      </c>
+      <c r="J147">
+        <v>309.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>8760</v>
+      </c>
+      <c r="B148">
+        <v>1031.4000000000001</v>
+      </c>
+      <c r="C148">
+        <v>969.28</v>
+      </c>
+      <c r="D148">
+        <v>801.11</v>
+      </c>
+      <c r="E148">
+        <v>639.83000000000004</v>
+      </c>
+      <c r="F148">
+        <v>639.83000000000004</v>
+      </c>
+      <c r="G148">
+        <v>524.9</v>
+      </c>
+      <c r="H148">
+        <v>432.55</v>
+      </c>
+      <c r="I148">
+        <v>369.48</v>
+      </c>
+      <c r="J148">
+        <v>312.42</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>8820</v>
+      </c>
+      <c r="B149">
+        <v>1032.5999999999999</v>
+      </c>
+      <c r="C149">
+        <v>970.82</v>
+      </c>
+      <c r="D149">
+        <v>803.28</v>
+      </c>
+      <c r="E149">
+        <v>642.35</v>
+      </c>
+      <c r="F149">
+        <v>642.35</v>
+      </c>
+      <c r="G149">
+        <v>527.59</v>
+      </c>
+      <c r="H149">
+        <v>435.33</v>
+      </c>
+      <c r="I149">
+        <v>372.31</v>
+      </c>
+      <c r="J149">
+        <v>315.31</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>8880</v>
+      </c>
+      <c r="B150">
+        <v>1033.8</v>
+      </c>
+      <c r="C150">
+        <v>972.34</v>
+      </c>
+      <c r="D150">
+        <v>805.43</v>
+      </c>
+      <c r="E150">
+        <v>644.86</v>
+      </c>
+      <c r="F150">
+        <v>644.86</v>
+      </c>
+      <c r="G150">
+        <v>530.27</v>
+      </c>
+      <c r="H150">
+        <v>438.1</v>
+      </c>
+      <c r="I150">
+        <v>375.12</v>
+      </c>
+      <c r="J150">
+        <v>318.19</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>8940</v>
+      </c>
+      <c r="B151">
+        <v>1035</v>
+      </c>
+      <c r="C151">
+        <v>973.84</v>
+      </c>
+      <c r="D151">
+        <v>807.56</v>
+      </c>
+      <c r="E151">
+        <v>647.35</v>
+      </c>
+      <c r="F151">
+        <v>647.35</v>
+      </c>
+      <c r="G151">
+        <v>532.92999999999995</v>
+      </c>
+      <c r="H151">
+        <v>440.85</v>
+      </c>
+      <c r="I151">
+        <v>377.92</v>
+      </c>
+      <c r="J151">
+        <v>321.05</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>9000</v>
+      </c>
+      <c r="B152">
+        <v>1036.2</v>
+      </c>
+      <c r="C152">
+        <v>975.34</v>
+      </c>
+      <c r="D152">
+        <v>809.68</v>
+      </c>
+      <c r="E152">
+        <v>649.83000000000004</v>
+      </c>
+      <c r="F152">
+        <v>649.83000000000004</v>
+      </c>
+      <c r="G152">
+        <v>535.59</v>
+      </c>
+      <c r="H152">
+        <v>443.59</v>
+      </c>
+      <c r="I152">
+        <v>380.7</v>
+      </c>
+      <c r="J152">
+        <v>323.89</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>9060</v>
+      </c>
+      <c r="B153">
+        <v>1037.4000000000001</v>
+      </c>
+      <c r="C153">
+        <v>976.83</v>
+      </c>
+      <c r="D153">
+        <v>811.79</v>
+      </c>
+      <c r="E153">
+        <v>652.29999999999995</v>
+      </c>
+      <c r="F153">
+        <v>652.29999999999995</v>
+      </c>
+      <c r="G153">
+        <v>538.22</v>
+      </c>
+      <c r="H153">
+        <v>446.32</v>
+      </c>
+      <c r="I153">
+        <v>383.48</v>
+      </c>
+      <c r="J153">
+        <v>326.72000000000003</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>9120</v>
+      </c>
+      <c r="B154">
+        <v>1038.5999999999999</v>
+      </c>
+      <c r="C154">
+        <v>978.3</v>
+      </c>
+      <c r="D154">
+        <v>813.88</v>
+      </c>
+      <c r="E154">
+        <v>654.76</v>
+      </c>
+      <c r="F154">
+        <v>654.76</v>
+      </c>
+      <c r="G154">
+        <v>540.85</v>
+      </c>
+      <c r="H154">
+        <v>449.04</v>
+      </c>
+      <c r="I154">
+        <v>386.24</v>
+      </c>
+      <c r="J154">
+        <v>329.53</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>9180</v>
+      </c>
+      <c r="B155">
+        <v>1039.8</v>
+      </c>
+      <c r="C155">
+        <v>979.77</v>
+      </c>
+      <c r="D155">
+        <v>815.97</v>
+      </c>
+      <c r="E155">
+        <v>657.2</v>
+      </c>
+      <c r="F155">
+        <v>657.2</v>
+      </c>
+      <c r="G155">
+        <v>543.47</v>
+      </c>
+      <c r="H155">
+        <v>451.75</v>
+      </c>
+      <c r="I155">
+        <v>388.98</v>
+      </c>
+      <c r="J155">
+        <v>332.32</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>9240</v>
+      </c>
+      <c r="B156">
+        <v>1041</v>
+      </c>
+      <c r="C156">
+        <v>981.22</v>
+      </c>
+      <c r="D156">
+        <v>818.03</v>
+      </c>
+      <c r="E156">
+        <v>659.63</v>
+      </c>
+      <c r="F156">
+        <v>659.63</v>
+      </c>
+      <c r="G156">
+        <v>546.07000000000005</v>
+      </c>
+      <c r="H156">
+        <v>454.44</v>
+      </c>
+      <c r="I156">
+        <v>391.72</v>
+      </c>
+      <c r="J156">
+        <v>335.1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>9300</v>
+      </c>
+      <c r="B157">
+        <v>1042.0999999999999</v>
+      </c>
+      <c r="C157">
+        <v>982.67</v>
+      </c>
+      <c r="D157">
+        <v>820.09</v>
+      </c>
+      <c r="E157">
+        <v>662.05</v>
+      </c>
+      <c r="F157">
+        <v>662.05</v>
+      </c>
+      <c r="G157">
+        <v>548.66</v>
+      </c>
+      <c r="H157">
+        <v>457.12</v>
+      </c>
+      <c r="I157">
+        <v>394.45</v>
+      </c>
+      <c r="J157">
+        <v>337.87</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>9360</v>
+      </c>
+      <c r="B158">
+        <v>1043.3</v>
+      </c>
+      <c r="C158">
+        <v>984.1</v>
+      </c>
+      <c r="D158">
+        <v>822.13</v>
+      </c>
+      <c r="E158">
+        <v>664.46</v>
+      </c>
+      <c r="F158">
+        <v>664.46</v>
+      </c>
+      <c r="G158">
+        <v>551.24</v>
+      </c>
+      <c r="H158">
+        <v>459.79</v>
+      </c>
+      <c r="I158">
+        <v>397.16</v>
+      </c>
+      <c r="J158">
+        <v>340.62</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>9420</v>
+      </c>
+      <c r="B159">
+        <v>1044.4000000000001</v>
+      </c>
+      <c r="C159">
+        <v>985.52</v>
+      </c>
+      <c r="D159">
+        <v>824.15</v>
+      </c>
+      <c r="E159">
+        <v>666.85</v>
+      </c>
+      <c r="F159">
+        <v>666.85</v>
+      </c>
+      <c r="G159">
+        <v>553.80999999999995</v>
+      </c>
+      <c r="H159">
+        <v>462.45</v>
+      </c>
+      <c r="I159">
+        <v>399.86</v>
+      </c>
+      <c r="J159">
+        <v>343.35</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>9480</v>
+      </c>
+      <c r="B160">
+        <v>1045.5999999999999</v>
+      </c>
+      <c r="C160">
+        <v>986.94</v>
+      </c>
+      <c r="D160">
+        <v>826.17</v>
+      </c>
+      <c r="E160">
+        <v>669.23</v>
+      </c>
+      <c r="F160">
+        <v>669.23</v>
+      </c>
+      <c r="G160">
+        <v>556.36</v>
+      </c>
+      <c r="H160">
+        <v>465.1</v>
+      </c>
+      <c r="I160">
+        <v>402.55</v>
+      </c>
+      <c r="J160">
+        <v>346.07</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>9540</v>
+      </c>
+      <c r="B161">
+        <v>1046.7</v>
+      </c>
+      <c r="C161">
+        <v>988.34</v>
+      </c>
+      <c r="D161">
+        <v>828.17</v>
+      </c>
+      <c r="E161">
+        <v>671.6</v>
+      </c>
+      <c r="F161">
+        <v>671.6</v>
+      </c>
+      <c r="G161">
+        <v>558.91</v>
+      </c>
+      <c r="H161">
+        <v>467.74</v>
+      </c>
+      <c r="I161">
+        <v>405.23</v>
+      </c>
+      <c r="J161">
+        <v>348.78</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>9600</v>
+      </c>
+      <c r="B162">
+        <v>1047.8</v>
+      </c>
+      <c r="C162">
+        <v>989.74</v>
+      </c>
+      <c r="D162">
+        <v>830.16</v>
+      </c>
+      <c r="E162">
+        <v>673.96</v>
+      </c>
+      <c r="F162">
+        <v>673.96</v>
+      </c>
+      <c r="G162">
+        <v>561.44000000000005</v>
+      </c>
+      <c r="H162">
+        <v>470.36</v>
+      </c>
+      <c r="I162">
+        <v>407.9</v>
+      </c>
+      <c r="J162">
+        <v>351.47</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>9660</v>
+      </c>
+      <c r="B163">
+        <v>1048.9000000000001</v>
+      </c>
+      <c r="C163">
+        <v>991.12</v>
+      </c>
+      <c r="D163">
+        <v>832.14</v>
+      </c>
+      <c r="E163">
+        <v>676.31</v>
+      </c>
+      <c r="F163">
+        <v>676.31</v>
+      </c>
+      <c r="G163">
+        <v>563.96</v>
+      </c>
+      <c r="H163">
+        <v>472.98</v>
+      </c>
+      <c r="I163">
+        <v>410.56</v>
+      </c>
+      <c r="J163">
+        <v>354.15</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>9720</v>
+      </c>
+      <c r="B164">
+        <v>1050</v>
+      </c>
+      <c r="C164">
+        <v>992.5</v>
+      </c>
+      <c r="D164">
+        <v>834.11</v>
+      </c>
+      <c r="E164">
+        <v>678.65</v>
+      </c>
+      <c r="F164">
+        <v>678.65</v>
+      </c>
+      <c r="G164">
+        <v>566.47</v>
+      </c>
+      <c r="H164">
+        <v>475.58</v>
+      </c>
+      <c r="I164">
+        <v>413.2</v>
+      </c>
+      <c r="J164">
+        <v>356.82</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>9780</v>
+      </c>
+      <c r="B165">
+        <v>1051.0999999999999</v>
+      </c>
+      <c r="C165">
+        <v>993.86</v>
+      </c>
+      <c r="D165">
+        <v>836.06</v>
+      </c>
+      <c r="E165">
+        <v>680.97</v>
+      </c>
+      <c r="F165">
+        <v>680.97</v>
+      </c>
+      <c r="G165">
+        <v>568.97</v>
+      </c>
+      <c r="H165">
+        <v>478.17</v>
+      </c>
+      <c r="I165">
+        <v>415.84</v>
+      </c>
+      <c r="J165">
+        <v>359.47</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>9840</v>
+      </c>
+      <c r="B166">
+        <v>1052.2</v>
+      </c>
+      <c r="C166">
+        <v>995.22</v>
+      </c>
+      <c r="D166">
+        <v>838</v>
+      </c>
+      <c r="E166">
+        <v>683.28</v>
+      </c>
+      <c r="F166">
+        <v>683.28</v>
+      </c>
+      <c r="G166">
+        <v>571.46</v>
+      </c>
+      <c r="H166">
+        <v>480.76</v>
+      </c>
+      <c r="I166">
+        <v>418.46</v>
+      </c>
+      <c r="J166">
+        <v>362.11</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>9900</v>
+      </c>
+      <c r="B167">
+        <v>1053.3</v>
+      </c>
+      <c r="C167">
+        <v>996.57</v>
+      </c>
+      <c r="D167">
+        <v>839.93</v>
+      </c>
+      <c r="E167">
+        <v>685.59</v>
+      </c>
+      <c r="F167">
+        <v>685.59</v>
+      </c>
+      <c r="G167">
+        <v>573.92999999999995</v>
+      </c>
+      <c r="H167">
+        <v>483.33</v>
+      </c>
+      <c r="I167">
+        <v>421.07</v>
+      </c>
+      <c r="J167">
+        <v>364.74</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>9960</v>
+      </c>
+      <c r="B168">
+        <v>1054.3</v>
+      </c>
+      <c r="C168">
+        <v>997.9</v>
+      </c>
+      <c r="D168">
+        <v>841.85</v>
+      </c>
+      <c r="E168">
+        <v>687.88</v>
+      </c>
+      <c r="F168">
+        <v>687.88</v>
+      </c>
+      <c r="G168">
+        <v>576.4</v>
+      </c>
+      <c r="H168">
+        <v>485.89</v>
+      </c>
+      <c r="I168">
+        <v>423.68</v>
+      </c>
+      <c r="J168">
+        <v>367.36</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>10020</v>
+      </c>
+      <c r="B169">
+        <v>1055.4000000000001</v>
+      </c>
+      <c r="C169">
+        <v>999.23</v>
+      </c>
+      <c r="D169">
+        <v>843.76</v>
+      </c>
+      <c r="E169">
+        <v>690.16</v>
+      </c>
+      <c r="F169">
+        <v>690.16</v>
+      </c>
+      <c r="G169">
+        <v>578.85</v>
+      </c>
+      <c r="H169">
+        <v>488.44</v>
+      </c>
+      <c r="I169">
+        <v>426.27</v>
+      </c>
+      <c r="J169">
+        <v>369.96</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>10080</v>
+      </c>
+      <c r="B170">
+        <v>1056.5</v>
+      </c>
+      <c r="C170">
+        <v>1000.6</v>
+      </c>
+      <c r="D170">
+        <v>845.65</v>
+      </c>
+      <c r="E170">
+        <v>692.43</v>
+      </c>
+      <c r="F170">
+        <v>692.43</v>
+      </c>
+      <c r="G170">
+        <v>581.29999999999995</v>
+      </c>
+      <c r="H170">
+        <v>490.98</v>
+      </c>
+      <c r="I170">
+        <v>428.85</v>
+      </c>
+      <c r="J170">
+        <v>372.55</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>10140</v>
+      </c>
+      <c r="B171">
+        <v>1057.5</v>
+      </c>
+      <c r="C171">
+        <v>1001.9</v>
+      </c>
+      <c r="D171">
+        <v>847.54</v>
+      </c>
+      <c r="E171">
+        <v>694.69</v>
+      </c>
+      <c r="F171">
+        <v>694.69</v>
+      </c>
+      <c r="G171">
+        <v>583.73</v>
+      </c>
+      <c r="H171">
+        <v>493.51</v>
+      </c>
+      <c r="I171">
+        <v>431.41</v>
+      </c>
+      <c r="J171">
+        <v>375.13</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>10200</v>
+      </c>
+      <c r="B172">
+        <v>1058.5999999999999</v>
+      </c>
+      <c r="C172">
+        <v>1003.2</v>
+      </c>
+      <c r="D172">
+        <v>849.41</v>
+      </c>
+      <c r="E172">
+        <v>696.93</v>
+      </c>
+      <c r="F172">
+        <v>696.93</v>
+      </c>
+      <c r="G172">
+        <v>586.16</v>
+      </c>
+      <c r="H172">
+        <v>496.03</v>
+      </c>
+      <c r="I172">
+        <v>433.97</v>
+      </c>
+      <c r="J172">
+        <v>377.7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>10260</v>
+      </c>
+      <c r="B173">
+        <v>1059.5999999999999</v>
+      </c>
+      <c r="C173">
+        <v>1004.5</v>
+      </c>
+      <c r="D173">
+        <v>851.27</v>
+      </c>
+      <c r="E173">
+        <v>699.17</v>
+      </c>
+      <c r="F173">
+        <v>699.17</v>
+      </c>
+      <c r="G173">
+        <v>588.57000000000005</v>
+      </c>
+      <c r="H173">
+        <v>498.54</v>
+      </c>
+      <c r="I173">
+        <v>436.52</v>
+      </c>
+      <c r="J173">
+        <v>380.26</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>10320</v>
+      </c>
+      <c r="B174">
+        <v>1060.5999999999999</v>
+      </c>
+      <c r="C174">
+        <v>1005.7</v>
+      </c>
+      <c r="D174">
+        <v>853.12</v>
+      </c>
+      <c r="E174">
+        <v>701.4</v>
+      </c>
+      <c r="F174">
+        <v>701.4</v>
+      </c>
+      <c r="G174">
+        <v>590.98</v>
+      </c>
+      <c r="H174">
+        <v>501.05</v>
+      </c>
+      <c r="I174">
+        <v>439.06</v>
+      </c>
+      <c r="J174">
+        <v>382.8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>10380</v>
+      </c>
+      <c r="B175">
+        <v>1061.7</v>
+      </c>
+      <c r="C175">
+        <v>1007</v>
+      </c>
+      <c r="D175">
+        <v>854.96</v>
+      </c>
+      <c r="E175">
+        <v>703.61</v>
+      </c>
+      <c r="F175">
+        <v>703.61</v>
+      </c>
+      <c r="G175">
+        <v>593.37</v>
+      </c>
+      <c r="H175">
+        <v>503.54</v>
+      </c>
+      <c r="I175">
+        <v>441.59</v>
+      </c>
+      <c r="J175">
+        <v>385.34</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>10440</v>
+      </c>
+      <c r="B176">
+        <v>1062.7</v>
+      </c>
+      <c r="C176">
+        <v>1008.3</v>
+      </c>
+      <c r="D176">
+        <v>856.79</v>
+      </c>
+      <c r="E176">
+        <v>705.82</v>
+      </c>
+      <c r="F176">
+        <v>705.82</v>
+      </c>
+      <c r="G176">
+        <v>595.75</v>
+      </c>
+      <c r="H176">
+        <v>506.02</v>
+      </c>
+      <c r="I176">
+        <v>444.11</v>
+      </c>
+      <c r="J176">
+        <v>387.87</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>10500</v>
+      </c>
+      <c r="B177">
+        <v>1063.7</v>
+      </c>
+      <c r="C177">
+        <v>1009.5</v>
+      </c>
+      <c r="D177">
+        <v>858.61</v>
+      </c>
+      <c r="E177">
+        <v>708.01</v>
+      </c>
+      <c r="F177">
+        <v>708.01</v>
+      </c>
+      <c r="G177">
+        <v>598.13</v>
+      </c>
+      <c r="H177">
+        <v>508.49</v>
+      </c>
+      <c r="I177">
+        <v>446.61</v>
+      </c>
+      <c r="J177">
+        <v>390.38</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>10560</v>
+      </c>
+      <c r="B178">
+        <v>1064.7</v>
+      </c>
+      <c r="C178">
+        <v>1010.8</v>
+      </c>
+      <c r="D178">
+        <v>860.42</v>
+      </c>
+      <c r="E178">
+        <v>710.2</v>
+      </c>
+      <c r="F178">
+        <v>710.2</v>
+      </c>
+      <c r="G178">
+        <v>600.49</v>
+      </c>
+      <c r="H178">
+        <v>510.94</v>
+      </c>
+      <c r="I178">
+        <v>449.11</v>
+      </c>
+      <c r="J178">
+        <v>392.89</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>10620</v>
+      </c>
+      <c r="B179">
+        <v>1065.7</v>
+      </c>
+      <c r="C179">
+        <v>1012</v>
+      </c>
+      <c r="D179">
+        <v>862.22</v>
+      </c>
+      <c r="E179">
+        <v>712.37</v>
+      </c>
+      <c r="F179">
+        <v>712.37</v>
+      </c>
+      <c r="G179">
+        <v>602.84</v>
+      </c>
+      <c r="H179">
+        <v>513.39</v>
+      </c>
+      <c r="I179">
+        <v>451.6</v>
+      </c>
+      <c r="J179">
+        <v>395.39</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>10680</v>
+      </c>
+      <c r="B180">
+        <v>1066.7</v>
+      </c>
+      <c r="C180">
+        <v>1013.3</v>
+      </c>
+      <c r="D180">
+        <v>864.01</v>
+      </c>
+      <c r="E180">
+        <v>714.53</v>
+      </c>
+      <c r="F180">
+        <v>714.53</v>
+      </c>
+      <c r="G180">
+        <v>605.19000000000005</v>
+      </c>
+      <c r="H180">
+        <v>515.83000000000004</v>
+      </c>
+      <c r="I180">
+        <v>454.08</v>
+      </c>
+      <c r="J180">
+        <v>397.88</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>10740</v>
+      </c>
+      <c r="B181">
+        <v>1067.5999999999999</v>
+      </c>
+      <c r="C181">
+        <v>1014.5</v>
+      </c>
+      <c r="D181">
+        <v>865.79</v>
+      </c>
+      <c r="E181">
+        <v>716.69</v>
+      </c>
+      <c r="F181">
+        <v>716.69</v>
+      </c>
+      <c r="G181">
+        <v>607.52</v>
+      </c>
+      <c r="H181">
+        <v>518.26</v>
+      </c>
+      <c r="I181">
+        <v>456.55</v>
+      </c>
+      <c r="J181">
+        <v>400.36</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>10800</v>
+      </c>
+      <c r="B182">
+        <v>1068.5999999999999</v>
+      </c>
+      <c r="C182">
+        <v>1015.7</v>
+      </c>
+      <c r="D182">
+        <v>867.56</v>
+      </c>
+      <c r="E182">
+        <v>718.83</v>
+      </c>
+      <c r="F182">
+        <v>718.83</v>
+      </c>
+      <c r="G182">
+        <v>609.84</v>
+      </c>
+      <c r="H182">
+        <v>520.67999999999995</v>
+      </c>
+      <c r="I182">
+        <v>459.01</v>
+      </c>
+      <c r="J182">
+        <v>402.83</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>10860</v>
+      </c>
+      <c r="B183">
+        <v>1069.5999999999999</v>
+      </c>
+      <c r="C183">
+        <v>1016.9</v>
+      </c>
+      <c r="D183">
+        <v>869.32</v>
+      </c>
+      <c r="E183">
+        <v>720.96</v>
+      </c>
+      <c r="F183">
+        <v>720.96</v>
+      </c>
+      <c r="G183">
+        <v>612.15</v>
+      </c>
+      <c r="H183">
+        <v>523.09</v>
+      </c>
+      <c r="I183">
+        <v>461.46</v>
+      </c>
+      <c r="J183">
+        <v>405.3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>10920</v>
+      </c>
+      <c r="B184">
+        <v>1070.5999999999999</v>
+      </c>
+      <c r="C184">
+        <v>1018.1</v>
+      </c>
+      <c r="D184">
+        <v>871.07</v>
+      </c>
+      <c r="E184">
+        <v>723.08</v>
+      </c>
+      <c r="F184">
+        <v>723.08</v>
+      </c>
+      <c r="G184">
+        <v>614.46</v>
+      </c>
+      <c r="H184">
+        <v>525.49</v>
+      </c>
+      <c r="I184">
+        <v>463.9</v>
+      </c>
+      <c r="J184">
+        <v>407.76</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>10980</v>
+      </c>
+      <c r="B185">
+        <v>1071.5</v>
+      </c>
+      <c r="C185">
+        <v>1019.3</v>
+      </c>
+      <c r="D185">
+        <v>872.8</v>
+      </c>
+      <c r="E185">
+        <v>725.19</v>
+      </c>
+      <c r="F185">
+        <v>725.19</v>
+      </c>
+      <c r="G185">
+        <v>616.75</v>
+      </c>
+      <c r="H185">
+        <v>527.88</v>
+      </c>
+      <c r="I185">
+        <v>466.33</v>
+      </c>
+      <c r="J185">
+        <v>410.21</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>11040</v>
+      </c>
+      <c r="B186">
+        <v>1072.5</v>
+      </c>
+      <c r="C186">
+        <v>1020.5</v>
+      </c>
+      <c r="D186">
+        <v>874.53</v>
+      </c>
+      <c r="E186">
+        <v>727.29</v>
+      </c>
+      <c r="F186">
+        <v>727.29</v>
+      </c>
+      <c r="G186">
+        <v>619.03</v>
+      </c>
+      <c r="H186">
+        <v>530.26</v>
+      </c>
+      <c r="I186">
+        <v>468.76</v>
+      </c>
+      <c r="J186">
+        <v>412.65</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>11100</v>
+      </c>
+      <c r="B187">
+        <v>1073.4000000000001</v>
+      </c>
+      <c r="C187">
+        <v>1021.7</v>
+      </c>
+      <c r="D187">
+        <v>876.26</v>
+      </c>
+      <c r="E187">
+        <v>729.38</v>
+      </c>
+      <c r="F187">
+        <v>729.38</v>
+      </c>
+      <c r="G187">
+        <v>621.30999999999995</v>
+      </c>
+      <c r="H187">
+        <v>532.63</v>
+      </c>
+      <c r="I187">
+        <v>471.17</v>
+      </c>
+      <c r="J187">
+        <v>415.09</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>11160</v>
+      </c>
+      <c r="B188">
+        <v>1074.3</v>
+      </c>
+      <c r="C188">
+        <v>1022.9</v>
+      </c>
+      <c r="D188">
+        <v>877.97</v>
+      </c>
+      <c r="E188">
+        <v>731.46</v>
+      </c>
+      <c r="F188">
+        <v>731.46</v>
+      </c>
+      <c r="G188">
+        <v>623.57000000000005</v>
+      </c>
+      <c r="H188">
+        <v>534.99</v>
+      </c>
+      <c r="I188">
+        <v>473.58</v>
+      </c>
+      <c r="J188">
+        <v>417.52</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>11220</v>
+      </c>
+      <c r="B189">
+        <v>1075.3</v>
+      </c>
+      <c r="C189">
+        <v>1024</v>
+      </c>
+      <c r="D189">
+        <v>879.67</v>
+      </c>
+      <c r="E189">
+        <v>733.53</v>
+      </c>
+      <c r="F189">
+        <v>733.53</v>
+      </c>
+      <c r="G189">
+        <v>625.82000000000005</v>
+      </c>
+      <c r="H189">
+        <v>537.34</v>
+      </c>
+      <c r="I189">
+        <v>475.98</v>
+      </c>
+      <c r="J189">
+        <v>419.94</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>11280</v>
+      </c>
+      <c r="B190">
+        <v>1076.2</v>
+      </c>
+      <c r="C190">
+        <v>1025.2</v>
+      </c>
+      <c r="D190">
+        <v>881.36</v>
+      </c>
+      <c r="E190">
+        <v>735.59</v>
+      </c>
+      <c r="F190">
+        <v>735.59</v>
+      </c>
+      <c r="G190">
+        <v>628.05999999999995</v>
+      </c>
+      <c r="H190">
+        <v>539.67999999999995</v>
+      </c>
+      <c r="I190">
+        <v>478.36</v>
+      </c>
+      <c r="J190">
+        <v>422.35</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>11340</v>
+      </c>
+      <c r="B191">
+        <v>1077.0999999999999</v>
+      </c>
+      <c r="C191">
+        <v>1026.3</v>
+      </c>
+      <c r="D191">
+        <v>883.04</v>
+      </c>
+      <c r="E191">
+        <v>737.64</v>
+      </c>
+      <c r="F191">
+        <v>737.64</v>
+      </c>
+      <c r="G191">
+        <v>630.29999999999995</v>
+      </c>
+      <c r="H191">
+        <v>542.01</v>
+      </c>
+      <c r="I191">
+        <v>480.75</v>
+      </c>
+      <c r="J191">
+        <v>424.76</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>11400</v>
+      </c>
+      <c r="B192">
+        <v>1078.0999999999999</v>
+      </c>
+      <c r="C192">
+        <v>1027.5</v>
+      </c>
+      <c r="D192">
+        <v>884.72</v>
+      </c>
+      <c r="E192">
+        <v>739.68</v>
+      </c>
+      <c r="F192">
+        <v>739.68</v>
+      </c>
+      <c r="G192">
+        <v>632.52</v>
+      </c>
+      <c r="H192">
+        <v>544.34</v>
+      </c>
+      <c r="I192">
+        <v>483.12</v>
+      </c>
+      <c r="J192">
+        <v>427.15</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>11460</v>
+      </c>
+      <c r="B193">
+        <v>1079</v>
+      </c>
+      <c r="C193">
+        <v>1028.5999999999999</v>
+      </c>
+      <c r="D193">
+        <v>886.39</v>
+      </c>
+      <c r="E193">
+        <v>741.71</v>
+      </c>
+      <c r="F193">
+        <v>741.71</v>
+      </c>
+      <c r="G193">
+        <v>634.73</v>
+      </c>
+      <c r="H193">
+        <v>546.65</v>
+      </c>
+      <c r="I193">
+        <v>485.48</v>
+      </c>
+      <c r="J193">
+        <v>429.55</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>11520</v>
+      </c>
+      <c r="B194">
+        <v>1079.9000000000001</v>
+      </c>
+      <c r="C194">
+        <v>1029.7</v>
+      </c>
+      <c r="D194">
+        <v>888.04</v>
+      </c>
+      <c r="E194">
+        <v>743.73</v>
+      </c>
+      <c r="F194">
+        <v>743.73</v>
+      </c>
+      <c r="G194">
+        <v>636.94000000000005</v>
+      </c>
+      <c r="H194">
+        <v>548.96</v>
+      </c>
+      <c r="I194">
+        <v>487.84</v>
+      </c>
+      <c r="J194">
+        <v>431.93</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>11580</v>
+      </c>
+      <c r="B195">
+        <v>1080.8</v>
+      </c>
+      <c r="C195">
+        <v>1030.9000000000001</v>
+      </c>
+      <c r="D195">
+        <v>889.69</v>
+      </c>
+      <c r="E195">
+        <v>745.74</v>
+      </c>
+      <c r="F195">
+        <v>745.74</v>
+      </c>
+      <c r="G195">
+        <v>639.13</v>
+      </c>
+      <c r="H195">
+        <v>551.25</v>
+      </c>
+      <c r="I195">
+        <v>490.19</v>
+      </c>
+      <c r="J195">
+        <v>434.3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>11640</v>
+      </c>
+      <c r="B196">
+        <v>1081.7</v>
+      </c>
+      <c r="C196">
+        <v>1032</v>
+      </c>
+      <c r="D196">
+        <v>891.33</v>
+      </c>
+      <c r="E196">
+        <v>747.75</v>
+      </c>
+      <c r="F196">
+        <v>747.75</v>
+      </c>
+      <c r="G196">
+        <v>641.32000000000005</v>
+      </c>
+      <c r="H196">
+        <v>553.54</v>
+      </c>
+      <c r="I196">
+        <v>492.53</v>
+      </c>
+      <c r="J196">
+        <v>436.67</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>11700</v>
+      </c>
+      <c r="B197">
+        <v>1082.5999999999999</v>
+      </c>
+      <c r="C197">
+        <v>1033.0999999999999</v>
+      </c>
+      <c r="D197">
+        <v>892.96</v>
+      </c>
+      <c r="E197">
+        <v>749.74</v>
+      </c>
+      <c r="F197">
+        <v>749.74</v>
+      </c>
+      <c r="G197">
+        <v>643.5</v>
+      </c>
+      <c r="H197">
+        <v>555.82000000000005</v>
+      </c>
+      <c r="I197">
+        <v>494.86</v>
+      </c>
+      <c r="J197">
+        <v>439.03</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>11760</v>
+      </c>
+      <c r="B198">
+        <v>1083.4000000000001</v>
+      </c>
+      <c r="C198">
+        <v>1034.2</v>
+      </c>
+      <c r="D198">
+        <v>894.58</v>
+      </c>
+      <c r="E198">
+        <v>751.72</v>
+      </c>
+      <c r="F198">
+        <v>751.72</v>
+      </c>
+      <c r="G198">
+        <v>645.66999999999996</v>
+      </c>
+      <c r="H198">
+        <v>558.09</v>
+      </c>
+      <c r="I198">
+        <v>497.18</v>
+      </c>
+      <c r="J198">
+        <v>441.38</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>11820</v>
+      </c>
+      <c r="B199">
+        <v>1084.3</v>
+      </c>
+      <c r="C199">
+        <v>1035.3</v>
+      </c>
+      <c r="D199">
+        <v>896.2</v>
+      </c>
+      <c r="E199">
+        <v>753.7</v>
+      </c>
+      <c r="F199">
+        <v>753.7</v>
+      </c>
+      <c r="G199">
+        <v>647.83000000000004</v>
+      </c>
+      <c r="H199">
+        <v>560.35</v>
+      </c>
+      <c r="I199">
+        <v>499.5</v>
+      </c>
+      <c r="J199">
+        <v>443.73</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>11880</v>
+      </c>
+      <c r="B200">
+        <v>1085.2</v>
+      </c>
+      <c r="C200">
+        <v>1036.4000000000001</v>
+      </c>
+      <c r="D200">
+        <v>897.8</v>
+      </c>
+      <c r="E200">
+        <v>755.66</v>
+      </c>
+      <c r="F200">
+        <v>755.66</v>
+      </c>
+      <c r="G200">
+        <v>649.98</v>
+      </c>
+      <c r="H200">
+        <v>562.61</v>
+      </c>
+      <c r="I200">
+        <v>501.81</v>
+      </c>
+      <c r="J200">
+        <v>446.07</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>11940</v>
+      </c>
+      <c r="B201">
+        <v>1086.0999999999999</v>
+      </c>
+      <c r="C201">
+        <v>1037.4000000000001</v>
+      </c>
+      <c r="D201">
+        <v>899.4</v>
+      </c>
+      <c r="E201">
+        <v>757.62</v>
+      </c>
+      <c r="F201">
+        <v>757.62</v>
+      </c>
+      <c r="G201">
+        <v>652.12</v>
+      </c>
+      <c r="H201">
+        <v>564.85</v>
+      </c>
+      <c r="I201">
+        <v>504.11</v>
+      </c>
+      <c r="J201">
+        <v>448.4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>12000</v>
+      </c>
+      <c r="B202">
+        <v>1086.9000000000001</v>
+      </c>
+      <c r="C202">
+        <v>1038.5</v>
+      </c>
+      <c r="D202">
+        <v>900.99</v>
+      </c>
+      <c r="E202">
+        <v>759.57</v>
+      </c>
+      <c r="F202">
+        <v>759.57</v>
+      </c>
+      <c r="G202">
+        <v>654.25</v>
+      </c>
+      <c r="H202">
+        <v>567.09</v>
+      </c>
+      <c r="I202">
+        <v>506.4</v>
+      </c>
+      <c r="J202">
+        <v>450.72</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>12060</v>
+      </c>
+      <c r="B203">
+        <v>1087.8</v>
+      </c>
+      <c r="C203">
+        <v>1039.5999999999999</v>
+      </c>
+      <c r="D203">
+        <v>902.57</v>
+      </c>
+      <c r="E203">
+        <v>761.51</v>
+      </c>
+      <c r="F203">
+        <v>761.51</v>
+      </c>
+      <c r="G203">
+        <v>656.37</v>
+      </c>
+      <c r="H203">
+        <v>569.32000000000005</v>
+      </c>
+      <c r="I203">
+        <v>508.68</v>
+      </c>
+      <c r="J203">
+        <v>453.03</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>12120</v>
+      </c>
+      <c r="B204">
+        <v>1088.7</v>
+      </c>
+      <c r="C204">
+        <v>1040.5999999999999</v>
+      </c>
+      <c r="D204">
+        <v>904.14</v>
+      </c>
+      <c r="E204">
+        <v>763.44</v>
+      </c>
+      <c r="F204">
+        <v>763.44</v>
+      </c>
+      <c r="G204">
+        <v>658.49</v>
+      </c>
+      <c r="H204">
+        <v>571.54</v>
+      </c>
+      <c r="I204">
+        <v>510.96</v>
+      </c>
+      <c r="J204">
+        <v>455.34</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>12180</v>
+      </c>
+      <c r="B205">
+        <v>1089.5</v>
+      </c>
+      <c r="C205">
+        <v>1041.7</v>
+      </c>
+      <c r="D205">
+        <v>905.7</v>
+      </c>
+      <c r="E205">
+        <v>765.36</v>
+      </c>
+      <c r="F205">
+        <v>765.36</v>
+      </c>
+      <c r="G205">
+        <v>660.6</v>
+      </c>
+      <c r="H205">
+        <v>573.75</v>
+      </c>
+      <c r="I205">
+        <v>513.23</v>
+      </c>
+      <c r="J205">
+        <v>457.64</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>12240</v>
+      </c>
+      <c r="B206">
+        <v>1090.4000000000001</v>
+      </c>
+      <c r="C206">
+        <v>1042.8</v>
+      </c>
+      <c r="D206">
+        <v>907.26</v>
+      </c>
+      <c r="E206">
+        <v>767.27</v>
+      </c>
+      <c r="F206">
+        <v>767.27</v>
+      </c>
+      <c r="G206">
+        <v>662.7</v>
+      </c>
+      <c r="H206">
+        <v>575.96</v>
+      </c>
+      <c r="I206">
+        <v>515.49</v>
+      </c>
+      <c r="J206">
+        <v>459.93</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>12300</v>
+      </c>
+      <c r="B207">
+        <v>1091.2</v>
+      </c>
+      <c r="C207">
+        <v>1043.8</v>
+      </c>
+      <c r="D207">
+        <v>908.8</v>
+      </c>
+      <c r="E207">
+        <v>769.18</v>
+      </c>
+      <c r="F207">
+        <v>769.18</v>
+      </c>
+      <c r="G207">
+        <v>664.79</v>
+      </c>
+      <c r="H207">
+        <v>578.15</v>
+      </c>
+      <c r="I207">
+        <v>517.74</v>
+      </c>
+      <c r="J207">
+        <v>462.22</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>12360</v>
+      </c>
+      <c r="B208">
+        <v>1092</v>
+      </c>
+      <c r="C208">
+        <v>1044.8</v>
+      </c>
+      <c r="D208">
+        <v>910.34</v>
+      </c>
+      <c r="E208">
+        <v>771.07</v>
+      </c>
+      <c r="F208">
+        <v>771.07</v>
+      </c>
+      <c r="G208">
+        <v>666.87</v>
+      </c>
+      <c r="H208">
+        <v>580.34</v>
+      </c>
+      <c r="I208">
+        <v>519.98</v>
+      </c>
+      <c r="J208">
+        <v>464.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>12420</v>
+      </c>
+      <c r="B209">
+        <v>1092.8</v>
+      </c>
+      <c r="C209">
+        <v>1045.9000000000001</v>
+      </c>
+      <c r="D209">
+        <v>911.87</v>
+      </c>
+      <c r="E209">
+        <v>772.96</v>
+      </c>
+      <c r="F209">
+        <v>772.96</v>
+      </c>
+      <c r="G209">
+        <v>668.94</v>
+      </c>
+      <c r="H209">
+        <v>582.52</v>
+      </c>
+      <c r="I209">
+        <v>522.22</v>
+      </c>
+      <c r="J209">
+        <v>466.77</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>12480</v>
+      </c>
+      <c r="B210">
+        <v>1093.5999999999999</v>
+      </c>
+      <c r="C210">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="D210">
+        <v>913.39</v>
+      </c>
+      <c r="E210">
+        <v>774.84</v>
+      </c>
+      <c r="F210">
+        <v>774.84</v>
+      </c>
+      <c r="G210">
+        <v>671.01</v>
+      </c>
+      <c r="H210">
+        <v>584.70000000000005</v>
+      </c>
+      <c r="I210">
+        <v>524.45000000000005</v>
+      </c>
+      <c r="J210">
+        <v>469.03</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>12540</v>
+      </c>
+      <c r="B211">
+        <v>1094.5</v>
+      </c>
+      <c r="C211">
+        <v>1047.9000000000001</v>
+      </c>
+      <c r="D211">
+        <v>914.9</v>
+      </c>
+      <c r="E211">
+        <v>776.71</v>
+      </c>
+      <c r="F211">
+        <v>776.71</v>
+      </c>
+      <c r="G211">
+        <v>673.07</v>
+      </c>
+      <c r="H211">
+        <v>586.86</v>
+      </c>
+      <c r="I211">
+        <v>526.66999999999996</v>
+      </c>
+      <c r="J211">
+        <v>471.28</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>12600</v>
+      </c>
+      <c r="B212">
+        <v>1095.3</v>
+      </c>
+      <c r="C212">
+        <v>1048.9000000000001</v>
+      </c>
+      <c r="D212">
+        <v>916.4</v>
+      </c>
+      <c r="E212">
+        <v>778.58</v>
+      </c>
+      <c r="F212">
+        <v>778.58</v>
+      </c>
+      <c r="G212">
+        <v>675.12</v>
+      </c>
+      <c r="H212">
+        <v>589.02</v>
+      </c>
+      <c r="I212">
+        <v>528.88</v>
+      </c>
+      <c r="J212">
+        <v>473.53</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>12660</v>
+      </c>
+      <c r="B213">
+        <v>1096</v>
+      </c>
+      <c r="C213">
+        <v>1049.9000000000001</v>
+      </c>
+      <c r="D213">
+        <v>917.9</v>
+      </c>
+      <c r="E213">
+        <v>780.43</v>
+      </c>
+      <c r="F213">
+        <v>780.43</v>
+      </c>
+      <c r="G213">
+        <v>677.16</v>
+      </c>
+      <c r="H213">
+        <v>591.17999999999995</v>
+      </c>
+      <c r="I213">
+        <v>531.08000000000004</v>
+      </c>
+      <c r="J213">
+        <v>475.77</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>12720</v>
+      </c>
+      <c r="B214">
+        <v>1096.8</v>
+      </c>
+      <c r="C214">
+        <v>1050.9000000000001</v>
+      </c>
+      <c r="D214">
+        <v>919.38</v>
+      </c>
+      <c r="E214">
+        <v>782.28</v>
+      </c>
+      <c r="F214">
+        <v>782.28</v>
+      </c>
+      <c r="G214">
+        <v>679.19</v>
+      </c>
+      <c r="H214">
+        <v>593.32000000000005</v>
+      </c>
+      <c r="I214">
+        <v>533.28</v>
+      </c>
+      <c r="J214">
+        <v>478.01</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>12780</v>
+      </c>
+      <c r="B215">
+        <v>1097.5999999999999</v>
+      </c>
+      <c r="C215">
+        <v>1051.9000000000001</v>
+      </c>
+      <c r="D215">
+        <v>920.86</v>
+      </c>
+      <c r="E215">
+        <v>784.12</v>
+      </c>
+      <c r="F215">
+        <v>784.12</v>
+      </c>
+      <c r="G215">
+        <v>681.22</v>
+      </c>
+      <c r="H215">
+        <v>595.46</v>
+      </c>
+      <c r="I215">
+        <v>535.47</v>
+      </c>
+      <c r="J215">
+        <v>480.24</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>12840</v>
+      </c>
+      <c r="B216">
+        <v>1098.4000000000001</v>
+      </c>
+      <c r="C216">
+        <v>1052.8</v>
+      </c>
+      <c r="D216">
+        <v>922.33</v>
+      </c>
+      <c r="E216">
+        <v>785.95</v>
+      </c>
+      <c r="F216">
+        <v>785.95</v>
+      </c>
+      <c r="G216">
+        <v>683.24</v>
+      </c>
+      <c r="H216">
+        <v>597.59</v>
+      </c>
+      <c r="I216">
+        <v>537.65</v>
+      </c>
+      <c r="J216">
+        <v>482.46</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>12900</v>
+      </c>
+      <c r="B217">
+        <v>1099.2</v>
+      </c>
+      <c r="C217">
+        <v>1053.8</v>
+      </c>
+      <c r="D217">
+        <v>923.79</v>
+      </c>
+      <c r="E217">
+        <v>787.77</v>
+      </c>
+      <c r="F217">
+        <v>787.77</v>
+      </c>
+      <c r="G217">
+        <v>685.25</v>
+      </c>
+      <c r="H217">
+        <v>599.71</v>
+      </c>
+      <c r="I217">
+        <v>539.82000000000005</v>
+      </c>
+      <c r="J217">
+        <v>484.67</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>12960</v>
+      </c>
+      <c r="B218">
+        <v>1099.9000000000001</v>
+      </c>
+      <c r="C218">
+        <v>1054.8</v>
+      </c>
+      <c r="D218">
+        <v>925.24</v>
+      </c>
+      <c r="E218">
+        <v>789.59</v>
+      </c>
+      <c r="F218">
+        <v>789.59</v>
+      </c>
+      <c r="G218">
+        <v>687.25</v>
+      </c>
+      <c r="H218">
+        <v>601.82000000000005</v>
+      </c>
+      <c r="I218">
+        <v>541.99</v>
+      </c>
+      <c r="J218">
+        <v>486.88</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>13020</v>
+      </c>
+      <c r="B219">
+        <v>1100.7</v>
+      </c>
+      <c r="C219">
+        <v>1055.7</v>
+      </c>
+      <c r="D219">
+        <v>926.69</v>
+      </c>
+      <c r="E219">
+        <v>791.4</v>
+      </c>
+      <c r="F219">
+        <v>791.4</v>
+      </c>
+      <c r="G219">
+        <v>689.25</v>
+      </c>
+      <c r="H219">
+        <v>603.92999999999995</v>
+      </c>
+      <c r="I219">
+        <v>544.15</v>
+      </c>
+      <c r="J219">
+        <v>489.08</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>13080</v>
+      </c>
+      <c r="B220">
+        <v>1101.5</v>
+      </c>
+      <c r="C220">
+        <v>1056.7</v>
+      </c>
+      <c r="D220">
+        <v>928.12</v>
+      </c>
+      <c r="E220">
+        <v>793.2</v>
+      </c>
+      <c r="F220">
+        <v>793.2</v>
+      </c>
+      <c r="G220">
+        <v>691.24</v>
+      </c>
+      <c r="H220">
+        <v>606.03</v>
+      </c>
+      <c r="I220">
+        <v>546.29999999999995</v>
+      </c>
+      <c r="J220">
+        <v>491.27</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>13140</v>
+      </c>
+      <c r="B221">
+        <v>1102.2</v>
+      </c>
+      <c r="C221">
+        <v>1057.5999999999999</v>
+      </c>
+      <c r="D221">
+        <v>929.55</v>
+      </c>
+      <c r="E221">
+        <v>794.99</v>
+      </c>
+      <c r="F221">
+        <v>794.99</v>
+      </c>
+      <c r="G221">
+        <v>693.22</v>
+      </c>
+      <c r="H221">
+        <v>608.12</v>
+      </c>
+      <c r="I221">
+        <v>548.45000000000005</v>
+      </c>
+      <c r="J221">
+        <v>493.45</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>13200</v>
+      </c>
+      <c r="B222">
+        <v>1103</v>
+      </c>
+      <c r="C222">
+        <v>1058.5999999999999</v>
+      </c>
+      <c r="D222">
+        <v>930.97</v>
+      </c>
+      <c r="E222">
+        <v>796.77</v>
+      </c>
+      <c r="F222">
+        <v>796.77</v>
+      </c>
+      <c r="G222">
+        <v>695.19</v>
+      </c>
+      <c r="H222">
+        <v>610.20000000000005</v>
+      </c>
+      <c r="I222">
+        <v>550.58000000000004</v>
+      </c>
+      <c r="J222">
+        <v>495.63</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>13260</v>
+      </c>
+      <c r="B223">
+        <v>1103.8</v>
+      </c>
+      <c r="C223">
+        <v>1059.5</v>
+      </c>
+      <c r="D223">
+        <v>932.38</v>
+      </c>
+      <c r="E223">
+        <v>798.55</v>
+      </c>
+      <c r="F223">
+        <v>798.55</v>
+      </c>
+      <c r="G223">
+        <v>697.16</v>
+      </c>
+      <c r="H223">
+        <v>612.28</v>
+      </c>
+      <c r="I223">
+        <v>552.71</v>
+      </c>
+      <c r="J223">
+        <v>497.81</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>13320</v>
+      </c>
+      <c r="B224">
+        <v>1104.5</v>
+      </c>
+      <c r="C224">
+        <v>1060.4000000000001</v>
+      </c>
+      <c r="D224">
+        <v>933.79</v>
+      </c>
+      <c r="E224">
+        <v>800.32</v>
+      </c>
+      <c r="F224">
+        <v>800.32</v>
+      </c>
+      <c r="G224">
+        <v>699.12</v>
+      </c>
+      <c r="H224">
+        <v>614.35</v>
+      </c>
+      <c r="I224">
+        <v>554.84</v>
+      </c>
+      <c r="J224">
+        <v>499.98</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>13380</v>
+      </c>
+      <c r="B225">
+        <v>1105.2</v>
+      </c>
+      <c r="C225">
+        <v>1061.4000000000001</v>
+      </c>
+      <c r="D225">
+        <v>935.18</v>
+      </c>
+      <c r="E225">
+        <v>802.08</v>
+      </c>
+      <c r="F225">
+        <v>802.08</v>
+      </c>
+      <c r="G225">
+        <v>701.07</v>
+      </c>
+      <c r="H225">
+        <v>616.41</v>
+      </c>
+      <c r="I225">
+        <v>556.95000000000005</v>
+      </c>
+      <c r="J225">
+        <v>502.14</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>13440</v>
+      </c>
+      <c r="B226">
+        <v>1106</v>
+      </c>
+      <c r="C226">
+        <v>1062.3</v>
+      </c>
+      <c r="D226">
+        <v>936.57</v>
+      </c>
+      <c r="E226">
+        <v>803.84</v>
+      </c>
+      <c r="F226">
+        <v>803.84</v>
+      </c>
+      <c r="G226">
+        <v>703.02</v>
+      </c>
+      <c r="H226">
+        <v>618.46</v>
+      </c>
+      <c r="I226">
+        <v>559.05999999999995</v>
+      </c>
+      <c r="J226">
+        <v>504.29</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>13500</v>
+      </c>
+      <c r="B227">
+        <v>1106.7</v>
+      </c>
+      <c r="C227">
+        <v>1063.2</v>
+      </c>
+      <c r="D227">
+        <v>937.96</v>
+      </c>
+      <c r="E227">
+        <v>805.58</v>
+      </c>
+      <c r="F227">
+        <v>805.58</v>
+      </c>
+      <c r="G227">
+        <v>704.95</v>
+      </c>
+      <c r="H227">
+        <v>620.51</v>
+      </c>
+      <c r="I227">
+        <v>561.16</v>
+      </c>
+      <c r="J227">
+        <v>506.44</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>13560</v>
+      </c>
+      <c r="B228">
+        <v>1107.5</v>
+      </c>
+      <c r="C228">
+        <v>1064.0999999999999</v>
+      </c>
+      <c r="D228">
+        <v>939.33</v>
+      </c>
+      <c r="E228">
+        <v>807.32</v>
+      </c>
+      <c r="F228">
+        <v>807.32</v>
+      </c>
+      <c r="G228">
+        <v>706.88</v>
+      </c>
+      <c r="H228">
+        <v>622.54999999999995</v>
+      </c>
+      <c r="I228">
+        <v>563.26</v>
+      </c>
+      <c r="J228">
+        <v>508.58</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>13620</v>
+      </c>
+      <c r="B229">
+        <v>1108.2</v>
+      </c>
+      <c r="C229">
+        <v>1065</v>
+      </c>
+      <c r="D229">
+        <v>940.7</v>
+      </c>
+      <c r="E229">
+        <v>809.06</v>
+      </c>
+      <c r="F229">
+        <v>809.06</v>
+      </c>
+      <c r="G229">
+        <v>708.8</v>
+      </c>
+      <c r="H229">
+        <v>624.58000000000004</v>
+      </c>
+      <c r="I229">
+        <v>565.35</v>
+      </c>
+      <c r="J229">
+        <v>510.71</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>13680</v>
+      </c>
+      <c r="B230">
+        <v>1108.9000000000001</v>
+      </c>
+      <c r="C230">
+        <v>1065.9000000000001</v>
+      </c>
+      <c r="D230">
+        <v>942.06</v>
+      </c>
+      <c r="E230">
+        <v>810.78</v>
+      </c>
+      <c r="F230">
+        <v>810.78</v>
+      </c>
+      <c r="G230">
+        <v>710.72</v>
+      </c>
+      <c r="H230">
+        <v>626.61</v>
+      </c>
+      <c r="I230">
+        <v>567.42999999999995</v>
+      </c>
+      <c r="J230">
+        <v>512.84</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>13740</v>
+      </c>
+      <c r="B231">
+        <v>1109.5999999999999</v>
+      </c>
+      <c r="C231">
+        <v>1066.8</v>
+      </c>
+      <c r="D231">
+        <v>943.42</v>
+      </c>
+      <c r="E231">
+        <v>812.49</v>
+      </c>
+      <c r="F231">
+        <v>812.49</v>
+      </c>
+      <c r="G231">
+        <v>712.63</v>
+      </c>
+      <c r="H231">
+        <v>628.62</v>
+      </c>
+      <c r="I231">
+        <v>569.5</v>
+      </c>
+      <c r="J231">
+        <v>514.96</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>13800</v>
+      </c>
+      <c r="B232">
+        <v>1110.4000000000001</v>
+      </c>
+      <c r="C232">
+        <v>1067.7</v>
+      </c>
+      <c r="D232">
+        <v>944.77</v>
+      </c>
+      <c r="E232">
+        <v>814.2</v>
+      </c>
+      <c r="F232">
+        <v>814.2</v>
+      </c>
+      <c r="G232">
+        <v>714.52</v>
+      </c>
+      <c r="H232">
+        <v>630.63</v>
+      </c>
+      <c r="I232">
+        <v>571.57000000000005</v>
+      </c>
+      <c r="J232">
+        <v>517.07000000000005</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>13860</v>
+      </c>
+      <c r="B233">
+        <v>1111.0999999999999</v>
+      </c>
+      <c r="C233">
+        <v>1068.5999999999999</v>
+      </c>
+      <c r="D233">
+        <v>946.11</v>
+      </c>
+      <c r="E233">
+        <v>815.9</v>
+      </c>
+      <c r="F233">
+        <v>815.9</v>
+      </c>
+      <c r="G233">
+        <v>716.42</v>
+      </c>
+      <c r="H233">
+        <v>632.64</v>
+      </c>
+      <c r="I233">
+        <v>573.63</v>
+      </c>
+      <c r="J233">
+        <v>519.17999999999995</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>13920</v>
+      </c>
+      <c r="B234">
+        <v>1111.8</v>
+      </c>
+      <c r="C234">
+        <v>1069.5</v>
+      </c>
+      <c r="D234">
+        <v>947.44</v>
+      </c>
+      <c r="E234">
+        <v>817.6</v>
+      </c>
+      <c r="F234">
+        <v>817.6</v>
+      </c>
+      <c r="G234">
+        <v>718.3</v>
+      </c>
+      <c r="H234">
+        <v>634.63</v>
+      </c>
+      <c r="I234">
+        <v>575.69000000000005</v>
+      </c>
+      <c r="J234">
+        <v>521.28</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>13980</v>
+      </c>
+      <c r="B235">
+        <v>1112.5</v>
+      </c>
+      <c r="C235">
+        <v>1070.4000000000001</v>
+      </c>
+      <c r="D235">
+        <v>948.77</v>
+      </c>
+      <c r="E235">
+        <v>819.28</v>
+      </c>
+      <c r="F235">
+        <v>819.28</v>
+      </c>
+      <c r="G235">
+        <v>720.18</v>
+      </c>
+      <c r="H235">
+        <v>636.62</v>
+      </c>
+      <c r="I235">
+        <v>577.74</v>
+      </c>
+      <c r="J235">
+        <v>523.37</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>14040</v>
+      </c>
+      <c r="B236">
+        <v>1113.2</v>
+      </c>
+      <c r="C236">
+        <v>1071.3</v>
+      </c>
+      <c r="D236">
+        <v>950.09</v>
+      </c>
+      <c r="E236">
+        <v>820.96</v>
+      </c>
+      <c r="F236">
+        <v>820.96</v>
+      </c>
+      <c r="G236">
+        <v>722.05</v>
+      </c>
+      <c r="H236">
+        <v>638.6</v>
+      </c>
+      <c r="I236">
+        <v>579.78</v>
+      </c>
+      <c r="J236">
+        <v>525.46</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>14100</v>
+      </c>
+      <c r="B237">
+        <v>1113.9000000000001</v>
+      </c>
+      <c r="C237">
+        <v>1072.2</v>
+      </c>
+      <c r="D237">
+        <v>951.4</v>
+      </c>
+      <c r="E237">
+        <v>822.63</v>
+      </c>
+      <c r="F237">
+        <v>822.63</v>
+      </c>
+      <c r="G237">
+        <v>723.91</v>
+      </c>
+      <c r="H237">
+        <v>640.58000000000004</v>
+      </c>
+      <c r="I237">
+        <v>581.82000000000005</v>
+      </c>
+      <c r="J237">
+        <v>527.54</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>14160</v>
+      </c>
+      <c r="B238">
+        <v>1114.5999999999999</v>
+      </c>
+      <c r="C238">
+        <v>1073</v>
+      </c>
+      <c r="D238">
+        <v>952.71</v>
+      </c>
+      <c r="E238">
+        <v>824.29</v>
+      </c>
+      <c r="F238">
+        <v>824.29</v>
+      </c>
+      <c r="G238">
+        <v>725.76</v>
+      </c>
+      <c r="H238">
+        <v>642.54999999999995</v>
+      </c>
+      <c r="I238">
+        <v>583.85</v>
+      </c>
+      <c r="J238">
+        <v>529.62</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>14220</v>
+      </c>
+      <c r="B239">
+        <v>1115.3</v>
+      </c>
+      <c r="C239">
+        <v>1073.9000000000001</v>
+      </c>
+      <c r="D239">
+        <v>954.01</v>
+      </c>
+      <c r="E239">
+        <v>825.95</v>
+      </c>
+      <c r="F239">
+        <v>825.95</v>
+      </c>
+      <c r="G239">
+        <v>727.61</v>
+      </c>
+      <c r="H239">
+        <v>644.51</v>
+      </c>
+      <c r="I239">
+        <v>585.87</v>
+      </c>
+      <c r="J239">
+        <v>531.67999999999995</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>14280</v>
+      </c>
+      <c r="B240">
+        <v>1116</v>
+      </c>
+      <c r="C240">
+        <v>1074.8</v>
+      </c>
+      <c r="D240">
+        <v>955.31</v>
+      </c>
+      <c r="E240">
+        <v>827.59</v>
+      </c>
+      <c r="F240">
+        <v>827.59</v>
+      </c>
+      <c r="G240">
+        <v>729.45</v>
+      </c>
+      <c r="H240">
+        <v>646.46</v>
+      </c>
+      <c r="I240">
+        <v>587.89</v>
+      </c>
+      <c r="J240">
+        <v>533.75</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>14340</v>
+      </c>
+      <c r="B241">
+        <v>1116.7</v>
+      </c>
+      <c r="C241">
+        <v>1075.5999999999999</v>
+      </c>
+      <c r="D241">
+        <v>956.6</v>
+      </c>
+      <c r="E241">
+        <v>829.24</v>
+      </c>
+      <c r="F241">
+        <v>829.24</v>
+      </c>
+      <c r="G241">
+        <v>731.29</v>
+      </c>
+      <c r="H241">
+        <v>648.41</v>
+      </c>
+      <c r="I241">
+        <v>589.9</v>
+      </c>
+      <c r="J241">
+        <v>535.79999999999995</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>14400</v>
+      </c>
+      <c r="B242">
+        <v>1117.4000000000001</v>
+      </c>
+      <c r="C242">
+        <v>1076.5</v>
+      </c>
+      <c r="D242">
+        <v>957.88</v>
+      </c>
+      <c r="E242">
+        <v>830.87</v>
+      </c>
+      <c r="F242">
+        <v>830.87</v>
+      </c>
+      <c r="G242">
+        <v>733.11</v>
+      </c>
+      <c r="H242">
+        <v>650.35</v>
+      </c>
+      <c r="I242">
+        <v>591.9</v>
+      </c>
+      <c r="J242">
+        <v>537.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>